<commit_message>
ICA1 data + solution micro task
</commit_message>
<xml_diff>
--- a/dataset-generators/flights/Topology.xlsx
+++ b/dataset-generators/flights/Topology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leonov\PCU\SymbolicComputation2304\SymbolicComputation2304\dataset-generators\flights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D686D596-501F-466E-B4B3-90704790897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCA2FCF-CB00-49FC-9F70-093B8E699886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{FC90DC62-A36D-437F-9491-0AD4335354D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FC90DC62-A36D-437F-9491-0AD4335354D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>#</t>
   </si>
@@ -48,88 +48,55 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Poznan</t>
-  </si>
-  <si>
-    <t>Gdansk</t>
-  </si>
-  <si>
     <t>Warsaw</t>
   </si>
   <si>
     <t>Krakov</t>
   </si>
   <si>
-    <t>Bratislava</t>
-  </si>
-  <si>
     <t>Budapest</t>
   </si>
   <si>
-    <t>Belgrade</t>
-  </si>
-  <si>
-    <t>Tirane</t>
-  </si>
-  <si>
     <t>Rijeka</t>
   </si>
   <si>
     <t>Zagreb</t>
   </si>
   <si>
-    <t>Graz</t>
-  </si>
-  <si>
     <t>Napoli</t>
   </si>
   <si>
     <t>Rome</t>
   </si>
   <si>
-    <t>Verona</t>
-  </si>
-  <si>
     <t>Innsbruck</t>
   </si>
   <si>
-    <t>Salzburg</t>
-  </si>
-  <si>
     <t>Vienna</t>
   </si>
   <si>
+    <t>Prague</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Munich</t>
+  </si>
+  <si>
+    <t>City 1</t>
+  </si>
+  <si>
+    <t>City 2</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
     <t>Brno</t>
-  </si>
-  <si>
-    <t>Prague</t>
-  </si>
-  <si>
-    <t>Dresden</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>Magdeburg</t>
-  </si>
-  <si>
-    <t>Hamburg</t>
-  </si>
-  <si>
-    <t>Munich</t>
-  </si>
-  <si>
-    <t>Frankfurt</t>
-  </si>
-  <si>
-    <t>City 1</t>
-  </si>
-  <si>
-    <t>City 2</t>
-  </si>
-  <si>
-    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -490,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089F927D-017C-4F69-9AE5-9523F44E1341}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +481,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -522,7 +489,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -530,7 +497,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -538,7 +505,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -546,170 +513,79 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5E3D28-D75F-4DA0-8149-23B8D4554AB0}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -735,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>